<commit_message>
Atribuição de tarefas Task10
</commit_message>
<xml_diff>
--- a/Planilha Organização Tarefas.xlsx
+++ b/Planilha Organização Tarefas.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GISELLE\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/37612d9d55d913cf/Desktop/projeto_integradorOficial/documentacao/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="12" documentId="11_2706763F0A69841AA3E206250DB27D4E4FAA8C64" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A470D06F-0077-4804-84B0-5A5F85461717}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8880"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bloco 02" sheetId="1" r:id="rId1"/>
@@ -17,17 +18,6 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mh5Ks4+mtfOQnaXufRUTzqKSoieFg=="/>
     </ext>
@@ -36,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="37">
   <si>
     <t>DISTRIBUIÇÃO DAS TAREFAS – PROJETO INTEGRADOR</t>
   </si>
@@ -158,7 +148,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9">
     <font>
       <sz val="11"/>
@@ -380,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -415,9 +405,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -425,19 +412,23 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -448,10 +439,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,7 +471,7 @@
         <xdr:cNvPr id="2" name="image4.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -518,7 +505,7 @@
         <xdr:cNvPr id="3" name="image3.png" descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -552,7 +539,7 @@
         <xdr:cNvPr id="4" name="image2.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -586,7 +573,7 @@
         <xdr:cNvPr id="5" name="image4.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -620,7 +607,7 @@
         <xdr:cNvPr id="6" name="image3.png" descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -654,7 +641,7 @@
         <xdr:cNvPr id="7" name="image5.png" descr="Forma&#10;&#10;Descrição gerada automaticamente com confiança média" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -688,7 +675,7 @@
         <xdr:cNvPr id="8" name="image2.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -722,7 +709,7 @@
         <xdr:cNvPr id="9" name="image4.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -756,7 +743,7 @@
         <xdr:cNvPr id="10" name="image3.png" descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -790,7 +777,7 @@
         <xdr:cNvPr id="11" name="image5.png" descr="Forma&#10;&#10;Descrição gerada automaticamente com confiança média" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -824,7 +811,7 @@
         <xdr:cNvPr id="12" name="image2.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -858,7 +845,7 @@
         <xdr:cNvPr id="13" name="image4.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -892,7 +879,7 @@
         <xdr:cNvPr id="14" name="image3.png" descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -926,7 +913,7 @@
         <xdr:cNvPr id="15" name="image5.png" descr="Forma&#10;&#10;Descrição gerada automaticamente com confiança média" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -960,7 +947,7 @@
         <xdr:cNvPr id="16" name="image2.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000010000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -994,7 +981,7 @@
         <xdr:cNvPr id="17" name="image4.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1028,7 +1015,7 @@
         <xdr:cNvPr id="18" name="image3.png" descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1062,7 +1049,7 @@
         <xdr:cNvPr id="19" name="image5.png" descr="Forma&#10;&#10;Descrição gerada automaticamente com confiança média" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1096,7 +1083,7 @@
         <xdr:cNvPr id="20" name="image2.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1130,7 +1117,7 @@
         <xdr:cNvPr id="21" name="image1.png" descr="Texto&#10;&#10;Descrição gerada automaticamente com confiança média">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000015000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1164,7 +1151,7 @@
         <xdr:cNvPr id="22" name="image4.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1198,7 +1185,7 @@
         <xdr:cNvPr id="23" name="image3.png" descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000017000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1232,7 +1219,7 @@
         <xdr:cNvPr id="24" name="image5.png" descr="Forma&#10;&#10;Descrição gerada automaticamente com confiança média" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1266,7 +1253,7 @@
         <xdr:cNvPr id="25" name="image2.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000019000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1300,7 +1287,7 @@
         <xdr:cNvPr id="26" name="image5.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1334,7 +1321,7 @@
         <xdr:cNvPr id="27" name="image4.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1372,7 +1359,7 @@
         <xdr:cNvPr id="28" name="image3.png" descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000017000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1410,7 +1397,7 @@
         <xdr:cNvPr id="29" name="image5.png" descr="Forma&#10;&#10;Descrição gerada automaticamente com confiança média" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1448,7 +1435,7 @@
         <xdr:cNvPr id="30" name="image2.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000019000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1488,7 +1475,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="31" name="image4.png"/>
+        <xdr:cNvPr id="31" name="image4.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1541,7 +1534,7 @@
         <xdr:cNvPr id="32" name="image4.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1579,7 +1572,7 @@
         <xdr:cNvPr id="33" name="image3.png" descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000017000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1617,7 +1610,7 @@
         <xdr:cNvPr id="34" name="image5.png" descr="Forma&#10;&#10;Descrição gerada automaticamente com confiança média" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1655,7 +1648,7 @@
         <xdr:cNvPr id="35" name="image2.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000019000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1695,7 +1688,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="36" name="image4.png"/>
+        <xdr:cNvPr id="36" name="image4.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1748,7 +1747,7 @@
         <xdr:cNvPr id="37" name="image4.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1786,7 +1785,7 @@
         <xdr:cNvPr id="38" name="image3.png" descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000017000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1824,7 +1823,7 @@
         <xdr:cNvPr id="39" name="image5.png" descr="Forma&#10;&#10;Descrição gerada automaticamente com confiança média" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1862,7 +1861,7 @@
         <xdr:cNvPr id="40" name="image2.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000019000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1902,7 +1901,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="41" name="image4.png"/>
+        <xdr:cNvPr id="41" name="image4.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1942,6 +1947,67 @@
     </xdr:pic>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>274320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="image4.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9738360" y="6385560"/>
+          <a:ext cx="335280" cy="822960"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1960,7 +2026,7 @@
         <xdr:cNvPr id="2" name="image4.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1994,7 +2060,7 @@
         <xdr:cNvPr id="3" name="image3.png" descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2028,7 +2094,7 @@
         <xdr:cNvPr id="4" name="image2.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2062,7 +2128,7 @@
         <xdr:cNvPr id="5" name="image4.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2096,7 +2162,7 @@
         <xdr:cNvPr id="6" name="image3.png" descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2130,7 +2196,7 @@
         <xdr:cNvPr id="7" name="image5.png" descr="Forma&#10;&#10;Descrição gerada automaticamente com confiança média" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2164,7 +2230,7 @@
         <xdr:cNvPr id="8" name="image2.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2198,7 +2264,7 @@
         <xdr:cNvPr id="9" name="image4.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2232,7 +2298,7 @@
         <xdr:cNvPr id="10" name="image3.png" descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2266,7 +2332,7 @@
         <xdr:cNvPr id="11" name="image5.png" descr="Forma&#10;&#10;Descrição gerada automaticamente com confiança média" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2300,7 +2366,7 @@
         <xdr:cNvPr id="12" name="image2.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2334,7 +2400,7 @@
         <xdr:cNvPr id="13" name="image4.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2368,7 +2434,7 @@
         <xdr:cNvPr id="14" name="image3.png" descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2402,7 +2468,7 @@
         <xdr:cNvPr id="15" name="image5.png" descr="Forma&#10;&#10;Descrição gerada automaticamente com confiança média" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2436,7 +2502,7 @@
         <xdr:cNvPr id="16" name="image2.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000010000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2470,7 +2536,7 @@
         <xdr:cNvPr id="17" name="image4.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2504,7 +2570,7 @@
         <xdr:cNvPr id="18" name="image3.png" descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2538,7 +2604,7 @@
         <xdr:cNvPr id="19" name="image5.png" descr="Forma&#10;&#10;Descrição gerada automaticamente com confiança média" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2572,7 +2638,7 @@
         <xdr:cNvPr id="20" name="image2.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2606,7 +2672,7 @@
         <xdr:cNvPr id="21" name="image1.png" descr="Texto&#10;&#10;Descrição gerada automaticamente com confiança média">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000015000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2640,7 +2706,7 @@
         <xdr:cNvPr id="22" name="image4.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2674,7 +2740,7 @@
         <xdr:cNvPr id="23" name="image3.png" descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000017000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2708,7 +2774,7 @@
         <xdr:cNvPr id="24" name="image5.png" descr="Forma&#10;&#10;Descrição gerada automaticamente com confiança média" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2742,7 +2808,7 @@
         <xdr:cNvPr id="25" name="image2.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000019000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2776,7 +2842,7 @@
         <xdr:cNvPr id="26" name="image4.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2810,7 +2876,7 @@
         <xdr:cNvPr id="27" name="image3.png" descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2844,7 +2910,7 @@
         <xdr:cNvPr id="28" name="image5.png" descr="Forma&#10;&#10;Descrição gerada automaticamente com confiança média" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2878,7 +2944,7 @@
         <xdr:cNvPr id="29" name="image2.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2912,7 +2978,7 @@
         <xdr:cNvPr id="30" name="image4.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2946,7 +3012,7 @@
         <xdr:cNvPr id="31" name="image3.png" descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2980,7 +3046,7 @@
         <xdr:cNvPr id="32" name="image5.png" descr="Forma&#10;&#10;Descrição gerada automaticamente com confiança média" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000020000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3014,7 +3080,7 @@
         <xdr:cNvPr id="33" name="image2.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000021000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000021000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3048,7 +3114,7 @@
         <xdr:cNvPr id="34" name="image5.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000022000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000022000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3269,34 +3335,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K59" sqref="K59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="46.140625" customWidth="1"/>
-    <col min="3" max="3" width="2.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
-    <col min="5" max="5" width="46.140625" customWidth="1"/>
-    <col min="6" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
-    <col min="8" max="8" width="46.140625" customWidth="1"/>
-    <col min="9" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="46.109375" customWidth="1"/>
+    <col min="3" max="3" width="2.88671875" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" customWidth="1"/>
+    <col min="5" max="5" width="46.109375" customWidth="1"/>
+    <col min="6" max="6" width="2.88671875" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" customWidth="1"/>
+    <col min="8" max="8" width="46.109375" customWidth="1"/>
+    <col min="9" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="21" customHeight="1">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3305,11 +3371,11 @@
       </c>
     </row>
     <row r="2" spans="1:26" ht="21" customHeight="1">
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
@@ -3317,7 +3383,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" ht="14.4">
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -3325,26 +3391,26 @@
       <c r="F3" s="5"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" ht="14.4">
       <c r="B4" s="4"/>
       <c r="E4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:26" ht="20.25">
-      <c r="A5" s="29" t="s">
+    <row r="5" spans="1:26" ht="21">
+      <c r="A5" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="D5" s="29" t="s">
+      <c r="B5" s="25"/>
+      <c r="D5" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="30"/>
-      <c r="G5" s="29" t="s">
+      <c r="E5" s="25"/>
+      <c r="G5" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="30"/>
-    </row>
-    <row r="6" spans="1:26" ht="20.25">
+      <c r="H5" s="25"/>
+    </row>
+    <row r="6" spans="1:26" ht="21">
       <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
@@ -3365,16 +3431,16 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A7" s="18"/>
-      <c r="B7" s="26"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="8"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="26" t="s">
+      <c r="D7" s="20"/>
+      <c r="E7" s="27" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="8"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="26" t="s">
+      <c r="G7" s="20"/>
+      <c r="H7" s="27" t="s">
         <v>10</v>
       </c>
       <c r="I7" s="8"/>
@@ -3397,14 +3463,14 @@
       <c r="Z7" s="8"/>
     </row>
     <row r="8" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="8"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
@@ -3425,14 +3491,14 @@
       <c r="Z8" s="8"/>
     </row>
     <row r="9" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="8"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="8"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -3453,14 +3519,14 @@
       <c r="Z9" s="8"/>
     </row>
     <row r="10" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="8"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
@@ -3481,142 +3547,142 @@
       <c r="Z10" s="8"/>
     </row>
     <row r="11" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A11" s="18"/>
-      <c r="B11" s="26"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="26" t="s">
+      <c r="A11" s="20"/>
+      <c r="B11" s="27"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="18"/>
-      <c r="H11" s="26" t="s">
+      <c r="G11" s="20"/>
+      <c r="H11" s="27" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
     </row>
     <row r="13" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
     </row>
     <row r="14" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-    </row>
-    <row r="15" spans="1:26" ht="20.25">
-      <c r="A15" s="21"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+    </row>
+    <row r="15" spans="1:26" ht="20.399999999999999">
+      <c r="A15" s="17"/>
       <c r="B15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="21"/>
+      <c r="D15" s="17"/>
       <c r="E15" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="21"/>
+      <c r="G15" s="17"/>
       <c r="H15" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="20.25">
-      <c r="A16" s="22"/>
+    <row r="16" spans="1:26" ht="20.399999999999999">
+      <c r="A16" s="18"/>
       <c r="B16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="22"/>
+      <c r="D16" s="18"/>
       <c r="E16" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="22"/>
+      <c r="G16" s="18"/>
       <c r="H16" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="20.25">
-      <c r="A17" s="22"/>
+    <row r="17" spans="1:8" ht="20.399999999999999">
+      <c r="A17" s="18"/>
       <c r="B17" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="22"/>
+      <c r="D17" s="18"/>
       <c r="E17" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="22"/>
+      <c r="G17" s="18"/>
       <c r="H17" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="20.25">
-      <c r="A18" s="22"/>
+    <row r="18" spans="1:8" ht="20.399999999999999">
+      <c r="A18" s="18"/>
       <c r="B18" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="22"/>
+      <c r="D18" s="18"/>
       <c r="E18" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="22"/>
+      <c r="G18" s="18"/>
       <c r="H18" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="20.25">
-      <c r="A19" s="23"/>
+    <row r="19" spans="1:8" ht="20.399999999999999">
+      <c r="A19" s="19"/>
       <c r="B19" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="23"/>
+      <c r="D19" s="19"/>
       <c r="E19" s="10"/>
-      <c r="G19" s="23"/>
+      <c r="G19" s="19"/>
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A20" s="18"/>
-      <c r="B20" s="26"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="26" t="s">
+      <c r="A20" s="20"/>
+      <c r="B20" s="27"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="G20" s="18"/>
-      <c r="H20" s="26" t="s">
+      <c r="G20" s="20"/>
+      <c r="H20" s="27" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
     </row>
     <row r="23" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1">
       <c r="B24" s="4"/>
@@ -3624,18 +3690,18 @@
       <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="30"/>
-      <c r="D25" s="29" t="s">
+      <c r="B25" s="25"/>
+      <c r="D25" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="30"/>
-      <c r="G25" s="29" t="s">
+      <c r="E25" s="25"/>
+      <c r="G25" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="H25" s="30"/>
+      <c r="H25" s="25"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1">
       <c r="A26" s="6" t="s">
@@ -3658,192 +3724,192 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A27" s="18"/>
-      <c r="B27" s="25" t="s">
+      <c r="A27" s="20"/>
+      <c r="B27" s="26" t="s">
         <v>14</v>
       </c>
       <c r="C27" s="8"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="25" t="s">
+      <c r="D27" s="20"/>
+      <c r="E27" s="26" t="s">
         <v>19</v>
       </c>
       <c r="F27" s="8"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="25" t="s">
+      <c r="G27" s="20"/>
+      <c r="H27" s="26" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A28" s="19"/>
-      <c r="B28" s="19"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="21"/>
       <c r="C28" s="8"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
       <c r="F28" s="8"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A29" s="19"/>
-      <c r="B29" s="19"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
       <c r="C29" s="8"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
       <c r="F29" s="8"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
     </row>
     <row r="30" spans="1:8" ht="36" customHeight="1">
-      <c r="A30" s="20"/>
-      <c r="B30" s="20"/>
+      <c r="A30" s="22"/>
+      <c r="B30" s="22"/>
       <c r="C30" s="8"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
       <c r="F30" s="8"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A31" s="18"/>
-      <c r="B31" s="26" t="s">
+      <c r="A31" s="20"/>
+      <c r="B31" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="18"/>
-      <c r="E31" s="25" t="s">
+      <c r="D31" s="20"/>
+      <c r="E31" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="G31" s="18"/>
-      <c r="H31" s="25" t="s">
+      <c r="G31" s="20"/>
+      <c r="H31" s="26" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A32" s="19"/>
-      <c r="B32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
+      <c r="A32" s="21"/>
+      <c r="B32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A33" s="19"/>
-      <c r="B33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
     </row>
     <row r="34" spans="1:8" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A34" s="20"/>
-      <c r="B34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="19"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
+      <c r="A34" s="22"/>
+      <c r="B34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="21"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A35" s="21"/>
+      <c r="A35" s="17"/>
       <c r="B35" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D35" s="21"/>
-      <c r="E35" s="15" t="s">
+      <c r="D35" s="17"/>
+      <c r="E35" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G35" s="21"/>
+      <c r="G35" s="17"/>
       <c r="H35" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A36" s="22"/>
+      <c r="A36" s="18"/>
       <c r="B36" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D36" s="22"/>
-      <c r="E36" s="15" t="s">
+      <c r="D36" s="18"/>
+      <c r="E36" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G36" s="22"/>
-      <c r="H36" s="15" t="s">
+      <c r="G36" s="18"/>
+      <c r="H36" s="14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A37" s="22"/>
+      <c r="A37" s="18"/>
       <c r="B37" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D37" s="22"/>
-      <c r="E37" s="16" t="s">
+      <c r="D37" s="18"/>
+      <c r="E37" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G37" s="22"/>
-      <c r="H37" s="16" t="s">
+      <c r="G37" s="18"/>
+      <c r="H37" s="15" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A38" s="22"/>
+      <c r="A38" s="18"/>
       <c r="B38" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D38" s="22"/>
-      <c r="E38" s="16" t="s">
+      <c r="D38" s="18"/>
+      <c r="E38" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="G38" s="22"/>
-      <c r="H38" s="16" t="s">
+      <c r="G38" s="18"/>
+      <c r="H38" s="15" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A39" s="23"/>
+      <c r="A39" s="19"/>
       <c r="B39" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D39" s="23"/>
-      <c r="E39" s="17"/>
-      <c r="G39" s="23"/>
-      <c r="H39" s="15"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="16"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="14"/>
     </row>
     <row r="40" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A40" s="18"/>
-      <c r="B40" s="25" t="s">
+      <c r="A40" s="20"/>
+      <c r="B40" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D40" s="18"/>
-      <c r="E40" s="24" t="s">
+      <c r="D40" s="20"/>
+      <c r="E40" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="G40" s="18"/>
-      <c r="H40" s="24" t="s">
+      <c r="G40" s="20"/>
+      <c r="H40" s="23" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A41" s="19"/>
-      <c r="B41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="19"/>
+      <c r="A41" s="21"/>
+      <c r="B41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
     </row>
     <row r="42" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A42" s="19"/>
-      <c r="B42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
+      <c r="A42" s="21"/>
+      <c r="B42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
     </row>
     <row r="43" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A43" s="20"/>
-      <c r="B43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
     </row>
     <row r="44" spans="1:8" ht="15.75" customHeight="1">
       <c r="B44" s="4"/>
@@ -3856,18 +3922,18 @@
       <c r="H45" s="4"/>
     </row>
     <row r="46" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A46" s="29" t="s">
+      <c r="A46" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="30"/>
-      <c r="D46" s="29" t="s">
+      <c r="B46" s="25"/>
+      <c r="D46" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E46" s="30"/>
-      <c r="G46" s="29" t="s">
+      <c r="E46" s="25"/>
+      <c r="G46" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="H46" s="30"/>
+      <c r="H46" s="25"/>
     </row>
     <row r="47" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
       <c r="A47" s="6" t="s">
@@ -3890,168 +3956,182 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A48" s="18"/>
-      <c r="B48" s="25" t="s">
+      <c r="A48" s="20"/>
+      <c r="B48" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D48" s="18"/>
-      <c r="E48" s="25" t="s">
+      <c r="D48" s="20"/>
+      <c r="E48" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G48" s="18"/>
-      <c r="H48" s="25"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="23" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="49" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A49" s="19"/>
-      <c r="B49" s="19"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="G49" s="19"/>
-      <c r="H49" s="19"/>
+      <c r="A49" s="21"/>
+      <c r="B49" s="21"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="21"/>
     </row>
     <row r="50" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A50" s="19"/>
-      <c r="B50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="G50" s="19"/>
-      <c r="H50" s="19"/>
+      <c r="A50" s="21"/>
+      <c r="B50" s="21"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="G50" s="21"/>
+      <c r="H50" s="21"/>
     </row>
     <row r="51" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A51" s="20"/>
-      <c r="B51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
+      <c r="A51" s="22"/>
+      <c r="B51" s="22"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="22"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="22"/>
     </row>
     <row r="52" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A52" s="18"/>
-      <c r="B52" s="25" t="s">
+      <c r="A52" s="20"/>
+      <c r="B52" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D52" s="18"/>
-      <c r="E52" s="25" t="s">
+      <c r="D52" s="20"/>
+      <c r="E52" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="G52" s="18"/>
-      <c r="H52" s="25"/>
-    </row>
-    <row r="53" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A53" s="19"/>
-      <c r="B53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="G53" s="19"/>
-      <c r="H53" s="19"/>
-    </row>
-    <row r="54" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A54" s="19"/>
-      <c r="B54" s="19"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="19"/>
-      <c r="G54" s="19"/>
-      <c r="H54" s="19"/>
-    </row>
-    <row r="55" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A55" s="20"/>
-      <c r="B55" s="20"/>
-      <c r="D55" s="20"/>
-      <c r="E55" s="20"/>
-      <c r="G55" s="20"/>
-      <c r="H55" s="20"/>
-    </row>
-    <row r="56" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A56" s="21"/>
-      <c r="B56" s="14" t="s">
+      <c r="G52" s="20"/>
+      <c r="H52" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D56" s="21"/>
-      <c r="E56" s="14" t="s">
+    </row>
+    <row r="53" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A53" s="21"/>
+      <c r="B53" s="21"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
+      <c r="G53" s="21"/>
+      <c r="H53" s="21"/>
+    </row>
+    <row r="54" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A54" s="21"/>
+      <c r="B54" s="21"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="21"/>
+      <c r="G54" s="21"/>
+      <c r="H54" s="21"/>
+    </row>
+    <row r="55" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A55" s="22"/>
+      <c r="B55" s="22"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="22"/>
+      <c r="G55" s="22"/>
+      <c r="H55" s="22"/>
+    </row>
+    <row r="56" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A56" s="17"/>
+      <c r="B56" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G56" s="21"/>
-      <c r="H56" s="13"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G56" s="17"/>
+      <c r="H56" s="15" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="57" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A57" s="22"/>
-      <c r="B57" s="15" t="s">
+      <c r="A57" s="18"/>
+      <c r="B57" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D57" s="22"/>
-      <c r="E57" s="15" t="s">
+      <c r="D57" s="18"/>
+      <c r="E57" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G57" s="22"/>
-      <c r="H57" s="15"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="15" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="58" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A58" s="22"/>
-      <c r="B58" s="16" t="s">
+      <c r="A58" s="18"/>
+      <c r="B58" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D58" s="22"/>
-      <c r="E58" s="16" t="s">
+      <c r="D58" s="18"/>
+      <c r="E58" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G58" s="22"/>
-      <c r="H58" s="16"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="15" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="59" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A59" s="22"/>
-      <c r="B59" s="16" t="s">
+      <c r="A59" s="18"/>
+      <c r="B59" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D59" s="22"/>
-      <c r="E59" s="16" t="s">
+      <c r="D59" s="18"/>
+      <c r="E59" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="G59" s="22"/>
-      <c r="H59" s="16"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="15" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="60" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A60" s="23"/>
-      <c r="B60" s="15"/>
-      <c r="D60" s="23"/>
-      <c r="E60" s="15"/>
-      <c r="G60" s="23"/>
-      <c r="H60" s="15"/>
+      <c r="A60" s="19"/>
+      <c r="B60" s="14"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="14"/>
+      <c r="G60" s="19"/>
+      <c r="H60" s="14"/>
     </row>
     <row r="61" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A61" s="18"/>
-      <c r="B61" s="24" t="s">
+      <c r="A61" s="20"/>
+      <c r="B61" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D61" s="18"/>
-      <c r="E61" s="24" t="s">
+      <c r="D61" s="20"/>
+      <c r="E61" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="G61" s="18"/>
-      <c r="H61" s="24"/>
+      <c r="G61" s="20"/>
+      <c r="H61" s="23" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="62" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A62" s="19"/>
-      <c r="B62" s="19"/>
-      <c r="D62" s="19"/>
-      <c r="E62" s="19"/>
-      <c r="G62" s="19"/>
-      <c r="H62" s="19"/>
+      <c r="A62" s="21"/>
+      <c r="B62" s="21"/>
+      <c r="D62" s="21"/>
+      <c r="E62" s="21"/>
+      <c r="G62" s="21"/>
+      <c r="H62" s="21"/>
     </row>
     <row r="63" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A63" s="19"/>
-      <c r="B63" s="19"/>
-      <c r="D63" s="19"/>
-      <c r="E63" s="19"/>
-      <c r="G63" s="19"/>
-      <c r="H63" s="19"/>
+      <c r="A63" s="21"/>
+      <c r="B63" s="21"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="21"/>
+      <c r="G63" s="21"/>
+      <c r="H63" s="21"/>
     </row>
     <row r="64" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A64" s="20"/>
-      <c r="B64" s="20"/>
-      <c r="D64" s="20"/>
-      <c r="E64" s="20"/>
-      <c r="G64" s="20"/>
-      <c r="H64" s="20"/>
+      <c r="A64" s="22"/>
+      <c r="B64" s="22"/>
+      <c r="D64" s="22"/>
+      <c r="E64" s="22"/>
+      <c r="G64" s="22"/>
+      <c r="H64" s="22"/>
     </row>
     <row r="65" spans="2:8" ht="15.75" customHeight="1">
       <c r="B65" s="4"/>
@@ -8735,31 +8815,37 @@
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="G56:G60"/>
-    <mergeCell ref="G61:G64"/>
-    <mergeCell ref="H61:H64"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="G48:G51"/>
-    <mergeCell ref="H48:H51"/>
-    <mergeCell ref="G52:G55"/>
-    <mergeCell ref="H52:H55"/>
-    <mergeCell ref="A56:A60"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="B61:B64"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="E52:E55"/>
-    <mergeCell ref="D56:D60"/>
-    <mergeCell ref="D61:D64"/>
-    <mergeCell ref="E61:E64"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="D15:D19"/>
+    <mergeCell ref="H40:H43"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A35:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="D35:D39"/>
+    <mergeCell ref="G35:G39"/>
+    <mergeCell ref="D40:D43"/>
+    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="G40:G43"/>
+    <mergeCell ref="G31:G34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="H31:H34"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="G20:G23"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="D11:D14"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="G11:G14"/>
     <mergeCell ref="H11:H14"/>
@@ -8776,91 +8862,84 @@
     <mergeCell ref="G27:G30"/>
     <mergeCell ref="A20:A23"/>
     <mergeCell ref="B20:B23"/>
-    <mergeCell ref="H31:H34"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="G20:G23"/>
-    <mergeCell ref="B1:F2"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="H7:H10"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="B52:B55"/>
     <mergeCell ref="D31:D34"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="D15:D19"/>
-    <mergeCell ref="H40:H43"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A35:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="D35:D39"/>
-    <mergeCell ref="G35:G39"/>
-    <mergeCell ref="D40:D43"/>
-    <mergeCell ref="E40:E43"/>
-    <mergeCell ref="G40:G43"/>
-    <mergeCell ref="G31:G34"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="A56:A60"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="E52:E55"/>
+    <mergeCell ref="D56:D60"/>
+    <mergeCell ref="D61:D64"/>
+    <mergeCell ref="E61:E64"/>
+    <mergeCell ref="G56:G60"/>
+    <mergeCell ref="G61:G64"/>
+    <mergeCell ref="H61:H64"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="G48:G51"/>
+    <mergeCell ref="H48:H51"/>
+    <mergeCell ref="G52:G55"/>
+    <mergeCell ref="H52:H55"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="46.140625" customWidth="1"/>
-    <col min="3" max="3" width="2.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
-    <col min="5" max="5" width="46.140625" customWidth="1"/>
-    <col min="6" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
-    <col min="8" max="8" width="46.140625" customWidth="1"/>
-    <col min="9" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="46.109375" customWidth="1"/>
+    <col min="3" max="3" width="2.88671875" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" customWidth="1"/>
+    <col min="5" max="5" width="46.109375" customWidth="1"/>
+    <col min="6" max="6" width="2.88671875" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" customWidth="1"/>
+    <col min="8" max="8" width="46.109375" customWidth="1"/>
+    <col min="9" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="21" customHeight="1">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="21" customHeight="1">
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" ht="14.4">
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -8868,26 +8947,26 @@
       <c r="F3" s="5"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" ht="14.4">
       <c r="B4" s="4"/>
       <c r="E4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:26" ht="20.25">
-      <c r="A5" s="29" t="s">
+    <row r="5" spans="1:26" ht="21">
+      <c r="A5" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="D5" s="29" t="s">
+      <c r="B5" s="25"/>
+      <c r="D5" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="30"/>
-      <c r="G5" s="29" t="s">
+      <c r="E5" s="25"/>
+      <c r="G5" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="30"/>
-    </row>
-    <row r="6" spans="1:26" ht="20.25">
+      <c r="H5" s="25"/>
+    </row>
+    <row r="6" spans="1:26" ht="21">
       <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
@@ -8908,14 +8987,14 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A7" s="18"/>
-      <c r="B7" s="26"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="8"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="26"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="27"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="26"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="27"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
@@ -8936,14 +9015,14 @@
       <c r="Z7" s="8"/>
     </row>
     <row r="8" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="8"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
@@ -8964,14 +9043,14 @@
       <c r="Z8" s="8"/>
     </row>
     <row r="9" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="8"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="8"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -8992,14 +9071,14 @@
       <c r="Z9" s="8"/>
     </row>
     <row r="10" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="8"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
@@ -9020,118 +9099,118 @@
       <c r="Z10" s="8"/>
     </row>
     <row r="11" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A11" s="18"/>
-      <c r="B11" s="26"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="26"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="26"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="27"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="27"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="27"/>
     </row>
     <row r="12" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
     </row>
     <row r="13" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
     </row>
     <row r="14" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-    </row>
-    <row r="15" spans="1:26" ht="20.25">
-      <c r="A15" s="21"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+    </row>
+    <row r="15" spans="1:26" ht="20.399999999999999">
+      <c r="A15" s="17"/>
       <c r="B15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="21"/>
+      <c r="D15" s="17"/>
       <c r="E15" s="9"/>
-      <c r="G15" s="21"/>
+      <c r="G15" s="17"/>
       <c r="H15" s="9"/>
     </row>
-    <row r="16" spans="1:26" ht="20.25">
-      <c r="A16" s="22"/>
+    <row r="16" spans="1:26" ht="20.399999999999999">
+      <c r="A16" s="18"/>
       <c r="B16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="22"/>
+      <c r="D16" s="18"/>
       <c r="E16" s="9"/>
-      <c r="G16" s="22"/>
+      <c r="G16" s="18"/>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="1:8" ht="20.25">
-      <c r="A17" s="22"/>
+    <row r="17" spans="1:8" ht="20.399999999999999">
+      <c r="A17" s="18"/>
       <c r="B17" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="22"/>
+      <c r="D17" s="18"/>
       <c r="E17" s="9"/>
-      <c r="G17" s="22"/>
+      <c r="G17" s="18"/>
       <c r="H17" s="9"/>
     </row>
-    <row r="18" spans="1:8" ht="20.25">
-      <c r="A18" s="22"/>
+    <row r="18" spans="1:8" ht="20.399999999999999">
+      <c r="A18" s="18"/>
       <c r="B18" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="22"/>
+      <c r="D18" s="18"/>
       <c r="E18" s="9"/>
-      <c r="G18" s="22"/>
+      <c r="G18" s="18"/>
       <c r="H18" s="9"/>
     </row>
-    <row r="19" spans="1:8" ht="20.25">
-      <c r="A19" s="23"/>
+    <row r="19" spans="1:8" ht="20.399999999999999">
+      <c r="A19" s="19"/>
       <c r="B19" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="23"/>
+      <c r="D19" s="19"/>
       <c r="E19" s="10"/>
-      <c r="G19" s="23"/>
+      <c r="G19" s="19"/>
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A20" s="18"/>
-      <c r="B20" s="26"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="26"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="26"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="27"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="27"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="27"/>
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
     </row>
     <row r="23" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1">
       <c r="B24" s="4"/>
@@ -9139,18 +9218,18 @@
       <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="30"/>
-      <c r="D25" s="29" t="s">
+      <c r="B25" s="25"/>
+      <c r="D25" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="E25" s="30"/>
-      <c r="G25" s="29" t="s">
+      <c r="E25" s="25"/>
+      <c r="G25" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="H25" s="30"/>
+      <c r="H25" s="25"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1">
       <c r="A26" s="6" t="s">
@@ -9173,158 +9252,158 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A27" s="18"/>
-      <c r="B27" s="26"/>
+      <c r="A27" s="20"/>
+      <c r="B27" s="27"/>
       <c r="C27" s="8"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="26"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="27"/>
       <c r="F27" s="8"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="26"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="27"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A28" s="19"/>
-      <c r="B28" s="19"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="21"/>
       <c r="C28" s="8"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
       <c r="F28" s="8"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A29" s="19"/>
-      <c r="B29" s="19"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
       <c r="C29" s="8"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
       <c r="F29" s="8"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
     </row>
     <row r="30" spans="1:8" ht="33" customHeight="1">
-      <c r="A30" s="20"/>
-      <c r="B30" s="20"/>
+      <c r="A30" s="22"/>
+      <c r="B30" s="22"/>
       <c r="C30" s="8"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
       <c r="F30" s="8"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
     </row>
     <row r="31" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A31" s="18"/>
-      <c r="B31" s="26"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="26"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="26"/>
+      <c r="A31" s="20"/>
+      <c r="B31" s="27"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="27"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="27"/>
     </row>
     <row r="32" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A32" s="19"/>
-      <c r="B32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
+      <c r="A32" s="21"/>
+      <c r="B32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A33" s="19"/>
-      <c r="B33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
     </row>
     <row r="34" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A34" s="20"/>
-      <c r="B34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
+      <c r="A34" s="22"/>
+      <c r="B34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A35" s="21"/>
+      <c r="A35" s="17"/>
       <c r="B35" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="21"/>
+      <c r="D35" s="17"/>
       <c r="E35" s="9"/>
-      <c r="G35" s="21"/>
+      <c r="G35" s="17"/>
       <c r="H35" s="9"/>
     </row>
     <row r="36" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A36" s="22"/>
+      <c r="A36" s="18"/>
       <c r="B36" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D36" s="22"/>
+      <c r="D36" s="18"/>
       <c r="E36" s="9"/>
-      <c r="G36" s="22"/>
+      <c r="G36" s="18"/>
       <c r="H36" s="9"/>
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A37" s="22"/>
+      <c r="A37" s="18"/>
       <c r="B37" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D37" s="22"/>
+      <c r="D37" s="18"/>
       <c r="E37" s="9"/>
-      <c r="G37" s="22"/>
+      <c r="G37" s="18"/>
       <c r="H37" s="9"/>
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A38" s="22"/>
+      <c r="A38" s="18"/>
       <c r="B38" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D38" s="22"/>
+      <c r="D38" s="18"/>
       <c r="E38" s="9"/>
-      <c r="G38" s="22"/>
+      <c r="G38" s="18"/>
       <c r="H38" s="9"/>
     </row>
     <row r="39" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A39" s="23"/>
+      <c r="A39" s="19"/>
       <c r="B39" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D39" s="23"/>
+      <c r="D39" s="19"/>
       <c r="E39" s="10"/>
-      <c r="G39" s="23"/>
+      <c r="G39" s="19"/>
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A40" s="18"/>
-      <c r="B40" s="26"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="26"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="26"/>
+      <c r="A40" s="20"/>
+      <c r="B40" s="27"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="27"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="27"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A41" s="19"/>
-      <c r="B41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="19"/>
+      <c r="A41" s="21"/>
+      <c r="B41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
     </row>
     <row r="42" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A42" s="19"/>
-      <c r="B42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
+      <c r="A42" s="21"/>
+      <c r="B42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
     </row>
     <row r="43" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A43" s="20"/>
-      <c r="B43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
     </row>
     <row r="44" spans="1:8" ht="15.75" customHeight="1">
       <c r="B44" s="4"/>
@@ -9332,14 +9411,14 @@
       <c r="H44" s="4"/>
     </row>
     <row r="45" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A45" s="29" t="s">
+      <c r="A45" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="30"/>
-      <c r="D45" s="29" t="s">
+      <c r="B45" s="25"/>
+      <c r="D45" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="E45" s="30"/>
+      <c r="E45" s="25"/>
       <c r="H45" s="4"/>
     </row>
     <row r="46" spans="1:8" ht="15.75" customHeight="1">
@@ -9358,136 +9437,136 @@
       <c r="H46" s="4"/>
     </row>
     <row r="47" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A47" s="18"/>
-      <c r="B47" s="26"/>
+      <c r="A47" s="20"/>
+      <c r="B47" s="27"/>
       <c r="C47" s="8"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="26"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="27"/>
       <c r="H47" s="4"/>
     </row>
     <row r="48" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A48" s="19"/>
-      <c r="B48" s="19"/>
+      <c r="A48" s="21"/>
+      <c r="B48" s="21"/>
       <c r="C48" s="8"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
       <c r="H48" s="4"/>
     </row>
     <row r="49" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A49" s="19"/>
-      <c r="B49" s="19"/>
+      <c r="A49" s="21"/>
+      <c r="B49" s="21"/>
       <c r="C49" s="8"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
       <c r="H49" s="4"/>
     </row>
     <row r="50" spans="1:8" ht="31.5" customHeight="1">
-      <c r="A50" s="20"/>
-      <c r="B50" s="20"/>
+      <c r="A50" s="22"/>
+      <c r="B50" s="22"/>
       <c r="C50" s="8"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="22"/>
       <c r="H50" s="4"/>
     </row>
     <row r="51" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A51" s="18"/>
-      <c r="B51" s="26"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="26"/>
+      <c r="A51" s="20"/>
+      <c r="B51" s="27"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="27"/>
       <c r="H51" s="4"/>
     </row>
     <row r="52" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A52" s="19"/>
-      <c r="B52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
+      <c r="A52" s="21"/>
+      <c r="B52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
       <c r="H52" s="4"/>
     </row>
     <row r="53" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A53" s="19"/>
-      <c r="B53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
+      <c r="A53" s="21"/>
+      <c r="B53" s="21"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
       <c r="H53" s="4"/>
     </row>
     <row r="54" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A54" s="20"/>
-      <c r="B54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
+      <c r="A54" s="22"/>
+      <c r="B54" s="22"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="22"/>
       <c r="H54" s="4"/>
     </row>
     <row r="55" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A55" s="21"/>
+      <c r="A55" s="17"/>
       <c r="B55" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D55" s="21"/>
+      <c r="D55" s="17"/>
       <c r="E55" s="9"/>
       <c r="H55" s="4"/>
     </row>
     <row r="56" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A56" s="22"/>
+      <c r="A56" s="18"/>
       <c r="B56" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D56" s="22"/>
+      <c r="D56" s="18"/>
       <c r="E56" s="9"/>
       <c r="H56" s="4"/>
     </row>
     <row r="57" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A57" s="22"/>
+      <c r="A57" s="18"/>
       <c r="B57" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D57" s="22"/>
+      <c r="D57" s="18"/>
       <c r="E57" s="9"/>
       <c r="H57" s="4"/>
     </row>
     <row r="58" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A58" s="22"/>
+      <c r="A58" s="18"/>
       <c r="B58" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D58" s="22"/>
+      <c r="D58" s="18"/>
       <c r="E58" s="9"/>
       <c r="H58" s="4"/>
     </row>
     <row r="59" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A59" s="23"/>
+      <c r="A59" s="19"/>
       <c r="B59" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D59" s="23"/>
+      <c r="D59" s="19"/>
       <c r="E59" s="10"/>
       <c r="H59" s="4"/>
     </row>
     <row r="60" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A60" s="18"/>
-      <c r="B60" s="26"/>
-      <c r="D60" s="18"/>
-      <c r="E60" s="26"/>
+      <c r="A60" s="20"/>
+      <c r="B60" s="27"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="27"/>
       <c r="H60" s="4"/>
     </row>
     <row r="61" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A61" s="19"/>
-      <c r="B61" s="19"/>
-      <c r="D61" s="19"/>
-      <c r="E61" s="19"/>
+      <c r="A61" s="21"/>
+      <c r="B61" s="21"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="21"/>
       <c r="H61" s="4"/>
     </row>
     <row r="62" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A62" s="19"/>
-      <c r="B62" s="19"/>
-      <c r="D62" s="19"/>
-      <c r="E62" s="19"/>
+      <c r="A62" s="21"/>
+      <c r="B62" s="21"/>
+      <c r="D62" s="21"/>
+      <c r="E62" s="21"/>
       <c r="H62" s="4"/>
     </row>
     <row r="63" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A63" s="20"/>
-      <c r="B63" s="20"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="20"/>
+      <c r="A63" s="22"/>
+      <c r="B63" s="22"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="22"/>
       <c r="H63" s="4"/>
     </row>
     <row r="64" spans="1:8" ht="15.75" customHeight="1">
@@ -14177,21 +14256,40 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="H31:H34"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="B51:B54"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="D35:D39"/>
-    <mergeCell ref="G35:G39"/>
-    <mergeCell ref="D40:D43"/>
-    <mergeCell ref="G40:G43"/>
-    <mergeCell ref="H40:H43"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="G31:G34"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="D60:D63"/>
+    <mergeCell ref="E60:E63"/>
+    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D47:D50"/>
+    <mergeCell ref="E47:E50"/>
+    <mergeCell ref="D51:D54"/>
+    <mergeCell ref="E51:E54"/>
+    <mergeCell ref="D55:D59"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="G20:G23"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="D15:D19"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="G7:G10"/>
     <mergeCell ref="G11:G14"/>
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="G15:G19"/>
@@ -14208,40 +14306,21 @@
     <mergeCell ref="H27:H30"/>
     <mergeCell ref="B31:B34"/>
     <mergeCell ref="E31:E34"/>
-    <mergeCell ref="B1:F2"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="H7:H10"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="D15:D19"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="G20:G23"/>
-    <mergeCell ref="H20:H23"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D60:D63"/>
-    <mergeCell ref="E60:E63"/>
-    <mergeCell ref="E40:E43"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D47:D50"/>
-    <mergeCell ref="E47:E50"/>
-    <mergeCell ref="D51:D54"/>
-    <mergeCell ref="E51:E54"/>
-    <mergeCell ref="D55:D59"/>
+    <mergeCell ref="H31:H34"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="D35:D39"/>
+    <mergeCell ref="G35:G39"/>
+    <mergeCell ref="D40:D43"/>
+    <mergeCell ref="G40:G43"/>
+    <mergeCell ref="H40:H43"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="G31:G34"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="E27:E30"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0" footer="0"/>

</xml_diff>